<commit_message>
does not work yet
</commit_message>
<xml_diff>
--- a/doc/communications_thoughts.xlsx
+++ b/doc/communications_thoughts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexr\Documents\Baja\2023-2024-Firmware\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2EF8904-1807-4B40-89E4-6B9AE19BC62F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44EE23FA-C647-417C-AFC2-1A77AFC176E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30525" yWindow="720" windowWidth="20895" windowHeight="11835" xr2:uid="{8A7B06E4-038D-436F-AE46-DA5528615279}"/>
+    <workbookView xWindow="1068" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{8A7B06E4-038D-436F-AE46-DA5528615279}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="65">
   <si>
     <t>client-&gt;server</t>
   </si>
@@ -188,9 +188,6 @@
     <t>server-&gt;rasbpi</t>
   </si>
   <si>
-    <t>BEGIN, END</t>
-  </si>
-  <si>
     <t>rasbpi-&gt;server</t>
   </si>
   <si>
@@ -216,6 +213,24 @@
   </si>
   <si>
     <t>rasbpi</t>
+  </si>
+  <si>
+    <t>STARTUP</t>
+  </si>
+  <si>
+    <t>ok, im here too</t>
+  </si>
+  <si>
+    <t>ok cool, talk to joe</t>
+  </si>
+  <si>
+    <t>ok, talking to yo mama</t>
+  </si>
+  <si>
+    <t>commands</t>
+  </si>
+  <si>
+    <t>BEGIN orEND</t>
   </si>
 </sst>
 </file>
@@ -269,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -279,10 +294,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -617,25 +628,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4F6168A-3713-47BF-9C3E-90F4564843A2}">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
-    <col min="3" max="8" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="3" max="8" width="26.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>26</v>
       </c>
@@ -655,7 +666,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C3" s="4" t="s">
         <v>0</v>
       </c>
@@ -675,7 +686,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -701,7 +712,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
@@ -724,7 +735,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
@@ -747,7 +758,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
@@ -770,13 +781,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>45</v>
       </c>
@@ -787,7 +798,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
         <v>1</v>
@@ -802,19 +813,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
-      <c r="C12" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>54</v>
-      </c>
+    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
         <v>24</v>
@@ -828,7 +838,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -843,7 +853,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
@@ -858,7 +868,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -873,7 +883,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -888,7 +898,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -903,7 +913,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
@@ -918,7 +928,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -933,7 +943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
@@ -945,21 +955,21 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
         <v>30</v>
       </c>
@@ -976,7 +986,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
@@ -991,7 +1001,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1006,7 +1016,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1" t="s">
@@ -1021,7 +1031,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1036,7 +1046,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -1045,13 +1055,13 @@
         <v>40</v>
       </c>
       <c r="G29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H29" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -1066,7 +1076,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
@@ -1081,12 +1091,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" t="s">
@@ -1096,7 +1106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1" t="s">
@@ -1111,10 +1121,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -1126,21 +1136,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C35" s="5"/>
-      <c r="D35" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D35" t="s">
+        <v>54</v>
+      </c>
       <c r="G35" t="s">
         <v>0</v>
       </c>
       <c r="H35" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E36" t="s">
         <v>39</v>
       </c>
@@ -1151,20 +1158,20 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G37" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H37" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G38" t="s">
         <v>6</v>
@@ -1173,9 +1180,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G39" t="s">
         <v>8</v>
@@ -1184,12 +1191,72 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G40" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>59</v>
+      </c>
+      <c r="D43" t="s">
+        <v>24</v>
+      </c>
+      <c r="G43" t="s">
+        <v>0</v>
+      </c>
+      <c r="H43" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="E44" t="s">
+        <v>25</v>
+      </c>
+      <c r="G44" t="s">
+        <v>6</v>
+      </c>
+      <c r="H44" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D45" t="s">
+        <v>60</v>
+      </c>
+      <c r="G45" t="s">
+        <v>0</v>
+      </c>
+      <c r="H45" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="E46" t="s">
+        <v>61</v>
+      </c>
+      <c r="G46" t="s">
+        <v>6</v>
+      </c>
+      <c r="H46" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D47" t="s">
+        <v>62</v>
+      </c>
+      <c r="G47" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C48" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>